<commit_message>
change to Tris-HCl (remove 10 nM)
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.19.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.19.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E369C5-F571-6345-8CBA-F6BEEBA4EDAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5967976E-7916-BD4F-9125-D1257D291933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="2760" windowWidth="46600" windowHeight="25180" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="2760" windowWidth="46600" windowHeight="25180" tabRatio="262" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -1635,9 +1635,6 @@
     <t>UDF/Sample Buffer</t>
   </si>
   <si>
-    <t>10 mM Tris-HCl</t>
-  </si>
-  <si>
     <t>Nuclease-free water</t>
   </si>
   <si>
@@ -2069,6 +2066,9 @@
   </si>
   <si>
     <t>cancer-capture-panels-11</t>
+  </si>
+  <si>
+    <t>Tris-HCl</t>
   </si>
 </sst>
 </file>
@@ -4543,7 +4543,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4587,7 +4587,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4629,7 +4629,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="2"/>
@@ -4647,7 +4647,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>24</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -4817,18 +4817,18 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13" customHeight="1"/>
     <row r="47" spans="1:5" ht="42" customHeight="1">
       <c r="A47" s="34" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="42" customHeight="1">
       <c r="A48" s="34" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18" customHeight="1">
@@ -4839,7 +4839,7 @@
     <row r="50" spans="1:1" ht="13" customHeight="1"/>
     <row r="51" spans="1:1" ht="42" customHeight="1">
       <c r="A51" s="34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="19" customHeight="1">
@@ -4902,7 +4902,7 @@
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="69" spans="1:1">
@@ -4967,8 +4967,8 @@
   </sheetPr>
   <dimension ref="A1:AH428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15:P52"/>
+    <sheetView showGridLines="0" topLeftCell="G16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5315,7 +5315,7 @@
       <c r="S9" s="223"/>
       <c r="T9" s="100"/>
       <c r="U9" s="227" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="V9" s="227"/>
       <c r="W9" s="100"/>
@@ -5433,10 +5433,10 @@
       </c>
       <c r="T11" s="114"/>
       <c r="U11" s="195" t="s">
+        <v>424</v>
+      </c>
+      <c r="V11" s="115" t="s">
         <v>425</v>
-      </c>
-      <c r="V11" s="115" t="s">
-        <v>426</v>
       </c>
       <c r="W11" s="114"/>
       <c r="X11" s="194" t="s">
@@ -5561,10 +5561,10 @@
       </c>
       <c r="T13" s="138"/>
       <c r="U13" s="140" t="s">
+        <v>426</v>
+      </c>
+      <c r="V13" s="140" t="s">
         <v>427</v>
-      </c>
-      <c r="V13" s="140" t="s">
-        <v>428</v>
       </c>
       <c r="W13" s="138"/>
       <c r="X13" s="140" t="s">
@@ -5635,7 +5635,7 @@
     </row>
     <row r="15" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="198" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B15" s="199" t="s">
         <v>37</v>
@@ -5647,7 +5647,7 @@
         <v>283</v>
       </c>
       <c r="E15" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F15" s="200" t="s">
         <v>15</v>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
@@ -5682,25 +5682,25 @@
         <v>298</v>
       </c>
       <c r="R15" s="198" t="s">
+        <v>441</v>
+      </c>
+      <c r="S15" s="206" t="s">
         <v>442</v>
-      </c>
-      <c r="S15" s="206" t="s">
-        <v>443</v>
       </c>
       <c r="T15" s="150"/>
       <c r="U15" s="61" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="V15" s="61">
         <v>1</v>
       </c>
       <c r="W15" s="150"/>
       <c r="X15" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="Y15" s="180"/>
       <c r="Z15" s="210" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AA15" s="211">
         <v>5</v>
@@ -5717,15 +5717,15 @@
       </c>
       <c r="AF15" s="152"/>
       <c r="AG15" s="58" t="s">
+        <v>437</v>
+      </c>
+      <c r="AH15" s="58" t="s">
         <v>438</v>
-      </c>
-      <c r="AH15" s="58" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B16" s="199" t="s">
         <v>37</v>
@@ -5737,7 +5737,7 @@
         <v>288</v>
       </c>
       <c r="E16" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F16" s="200" t="s">
         <v>16</v>
@@ -5771,14 +5771,14 @@
       <c r="S16" s="208"/>
       <c r="T16" s="150"/>
       <c r="U16" s="61" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="V16" s="61">
         <v>1</v>
       </c>
       <c r="W16" s="150"/>
       <c r="X16" s="209" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="Y16" s="180"/>
       <c r="Z16" s="212"/>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="17" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="198" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B17" s="199" t="s">
         <v>37</v>
@@ -5809,7 +5809,7 @@
         <v>284</v>
       </c>
       <c r="E17" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F17" s="200" t="s">
         <v>15</v>
@@ -5843,14 +5843,14 @@
       <c r="S17" s="208"/>
       <c r="T17" s="150"/>
       <c r="U17" s="61" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V17" s="61">
         <v>1</v>
       </c>
       <c r="W17" s="150"/>
       <c r="X17" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="Y17" s="180"/>
       <c r="Z17" s="212"/>
@@ -5867,7 +5867,7 @@
     </row>
     <row r="18" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="198" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B18" s="199" t="s">
         <v>37</v>
@@ -5879,7 +5879,7 @@
         <v>285</v>
       </c>
       <c r="E18" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F18" s="200" t="s">
         <v>77</v>
@@ -5904,7 +5904,7 @@
       <c r="N18" s="57"/>
       <c r="O18" s="149"/>
       <c r="P18" s="30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Q18" s="202" t="s">
         <v>77</v>
@@ -5916,7 +5916,7 @@
       <c r="V18" s="61"/>
       <c r="W18" s="150"/>
       <c r="X18" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y18" s="180"/>
       <c r="Z18" s="212"/>
@@ -5933,7 +5933,7 @@
     </row>
     <row r="19" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="198" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B19" s="199" t="s">
         <v>37</v>
@@ -5945,7 +5945,7 @@
         <v>286</v>
       </c>
       <c r="E19" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F19" s="200" t="s">
         <v>77</v>
@@ -5982,7 +5982,7 @@
       <c r="V19" s="61"/>
       <c r="W19" s="150"/>
       <c r="X19" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Y19" s="180"/>
       <c r="Z19" s="212"/>
@@ -5996,12 +5996,12 @@
       <c r="AF19" s="152"/>
       <c r="AG19" s="58"/>
       <c r="AH19" s="58" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="198" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B20" s="199" t="s">
         <v>37</v>
@@ -6013,7 +6013,7 @@
         <v>287</v>
       </c>
       <c r="E20" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F20" s="200" t="s">
         <v>77</v>
@@ -6050,7 +6050,7 @@
       <c r="V20" s="61"/>
       <c r="W20" s="150"/>
       <c r="X20" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y20" s="180"/>
       <c r="Z20" s="212"/>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="21" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="198" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B21" s="199" t="s">
         <v>37</v>
@@ -6079,7 +6079,7 @@
         <v>376</v>
       </c>
       <c r="E21" s="198" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F21" s="200" t="s">
         <v>77</v>
@@ -6116,7 +6116,7 @@
       <c r="V21" s="61"/>
       <c r="W21" s="150"/>
       <c r="X21" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y21" s="180"/>
       <c r="Z21" s="212"/>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="22" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="198" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B22" s="199" t="s">
         <v>37</v>
@@ -6142,10 +6142,10 @@
         <v>297</v>
       </c>
       <c r="D22" s="201" t="s">
+        <v>448</v>
+      </c>
+      <c r="E22" s="198" t="s">
         <v>449</v>
-      </c>
-      <c r="E22" s="198" t="s">
-        <v>450</v>
       </c>
       <c r="F22" s="200" t="s">
         <v>77</v>
@@ -6182,11 +6182,11 @@
       <c r="V22" s="61"/>
       <c r="W22" s="150"/>
       <c r="X22" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y22" s="180"/>
       <c r="Z22" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA22" s="211">
         <v>40</v>
@@ -6200,7 +6200,7 @@
     </row>
     <row r="23" spans="1:34" ht="25" customHeight="1">
       <c r="A23" s="198" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B23" s="199" t="s">
         <v>37</v>
@@ -6209,10 +6209,10 @@
         <v>297</v>
       </c>
       <c r="D23" s="201" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E23" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F23" s="200" t="s">
         <v>77</v>
@@ -6249,11 +6249,11 @@
       <c r="V23" s="61"/>
       <c r="W23" s="150"/>
       <c r="X23" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y23" s="180"/>
       <c r="Z23" s="173" t="s">
-        <v>392</v>
+        <v>513</v>
       </c>
       <c r="AA23" s="211">
         <v>45</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="24" spans="1:34" ht="25" customHeight="1">
       <c r="A24" s="198" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B24" s="199" t="s">
         <v>37</v>
@@ -6277,10 +6277,10 @@
         <v>297</v>
       </c>
       <c r="D24" s="201" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E24" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F24" s="200" t="s">
         <v>77</v>
@@ -6317,11 +6317,11 @@
       <c r="V24" s="61"/>
       <c r="W24" s="150"/>
       <c r="X24" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y24" s="180"/>
       <c r="Z24" s="196" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AA24" s="211">
         <v>50</v>
@@ -6336,7 +6336,7 @@
     </row>
     <row r="25" spans="1:34" ht="25" customHeight="1">
       <c r="A25" s="198" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B25" s="199" t="s">
         <v>37</v>
@@ -6345,10 +6345,10 @@
         <v>297</v>
       </c>
       <c r="D25" s="201" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E25" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F25" s="200" t="s">
         <v>77</v>
@@ -6385,7 +6385,7 @@
       <c r="V25" s="61"/>
       <c r="W25" s="150"/>
       <c r="X25" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y25" s="180"/>
       <c r="Z25" s="173" t="s">
@@ -6401,12 +6401,12 @@
       <c r="AF25" s="152"/>
       <c r="AG25" s="58"/>
       <c r="AH25" s="58" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="25" customHeight="1">
       <c r="A26" s="198" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B26" s="199" t="s">
         <v>37</v>
@@ -6415,10 +6415,10 @@
         <v>297</v>
       </c>
       <c r="D26" s="201" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E26" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F26" s="200" t="s">
         <v>77</v>
@@ -6455,11 +6455,11 @@
       <c r="V26" s="61"/>
       <c r="W26" s="150"/>
       <c r="X26" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y26" s="180"/>
       <c r="Z26" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA26" s="211">
         <v>60</v>
@@ -6474,7 +6474,7 @@
     </row>
     <row r="27" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="198" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B27" s="199" t="s">
         <v>37</v>
@@ -6483,10 +6483,10 @@
         <v>297</v>
       </c>
       <c r="D27" s="201" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E27" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F27" s="200" t="s">
         <v>77</v>
@@ -6523,11 +6523,11 @@
       <c r="V27" s="61"/>
       <c r="W27" s="150"/>
       <c r="X27" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y27" s="180"/>
       <c r="Z27" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA27" s="211">
         <v>65</v>
@@ -6542,7 +6542,7 @@
     </row>
     <row r="28" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="198" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B28" s="199" t="s">
         <v>37</v>
@@ -6551,10 +6551,10 @@
         <v>297</v>
       </c>
       <c r="D28" s="201" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E28" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F28" s="200" t="s">
         <v>77</v>
@@ -6591,11 +6591,11 @@
       <c r="V28" s="61"/>
       <c r="W28" s="150"/>
       <c r="X28" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y28" s="180"/>
       <c r="Z28" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA28" s="211">
         <v>70</v>
@@ -6610,7 +6610,7 @@
     </row>
     <row r="29" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="198" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B29" s="199" t="s">
         <v>37</v>
@@ -6619,10 +6619,10 @@
         <v>297</v>
       </c>
       <c r="D29" s="201" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E29" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F29" s="200" t="s">
         <v>77</v>
@@ -6659,11 +6659,11 @@
       <c r="V29" s="61"/>
       <c r="W29" s="150"/>
       <c r="X29" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y29" s="180"/>
       <c r="Z29" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA29" s="211">
         <v>75</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="30" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="198" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B30" s="199" t="s">
         <v>37</v>
@@ -6687,10 +6687,10 @@
         <v>297</v>
       </c>
       <c r="D30" s="201" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E30" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F30" s="200" t="s">
         <v>77</v>
@@ -6727,11 +6727,11 @@
       <c r="V30" s="61"/>
       <c r="W30" s="150"/>
       <c r="X30" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y30" s="180"/>
       <c r="Z30" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA30" s="211">
         <v>80</v>
@@ -6746,7 +6746,7 @@
     </row>
     <row r="31" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="198" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B31" s="199" t="s">
         <v>37</v>
@@ -6755,10 +6755,10 @@
         <v>297</v>
       </c>
       <c r="D31" s="201" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E31" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F31" s="200" t="s">
         <v>77</v>
@@ -6795,11 +6795,11 @@
       <c r="V31" s="61"/>
       <c r="W31" s="150"/>
       <c r="X31" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y31" s="180"/>
       <c r="Z31" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA31" s="211">
         <v>85</v>
@@ -6814,7 +6814,7 @@
     </row>
     <row r="32" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="198" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B32" s="199" t="s">
         <v>37</v>
@@ -6823,10 +6823,10 @@
         <v>297</v>
       </c>
       <c r="D32" s="201" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E32" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F32" s="200" t="s">
         <v>77</v>
@@ -6863,11 +6863,11 @@
       <c r="V32" s="61"/>
       <c r="W32" s="150"/>
       <c r="X32" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y32" s="180"/>
       <c r="Z32" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA32" s="211">
         <v>90</v>
@@ -6882,7 +6882,7 @@
     </row>
     <row r="33" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="198" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B33" s="199" t="s">
         <v>37</v>
@@ -6891,10 +6891,10 @@
         <v>297</v>
       </c>
       <c r="D33" s="201" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E33" s="198" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F33" s="200" t="s">
         <v>77</v>
@@ -6931,11 +6931,11 @@
       <c r="V33" s="61"/>
       <c r="W33" s="150"/>
       <c r="X33" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y33" s="180"/>
       <c r="Z33" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA33" s="211">
         <v>95</v>
@@ -6950,7 +6950,7 @@
     </row>
     <row r="34" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="198" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B34" s="199" t="s">
         <v>37</v>
@@ -6959,10 +6959,10 @@
         <v>297</v>
       </c>
       <c r="D34" s="201" t="s">
+        <v>473</v>
+      </c>
+      <c r="E34" s="198" t="s">
         <v>474</v>
-      </c>
-      <c r="E34" s="198" t="s">
-        <v>475</v>
       </c>
       <c r="F34" s="200" t="s">
         <v>77</v>
@@ -6999,11 +6999,11 @@
       <c r="V34" s="61"/>
       <c r="W34" s="150"/>
       <c r="X34" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y34" s="180"/>
       <c r="Z34" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA34" s="211">
         <v>100</v>
@@ -7018,7 +7018,7 @@
     </row>
     <row r="35" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="198" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B35" s="199" t="s">
         <v>37</v>
@@ -7027,10 +7027,10 @@
         <v>297</v>
       </c>
       <c r="D35" s="201" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E35" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F35" s="200" t="s">
         <v>77</v>
@@ -7067,11 +7067,11 @@
       <c r="V35" s="61"/>
       <c r="W35" s="150"/>
       <c r="X35" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y35" s="180"/>
       <c r="Z35" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA35" s="211">
         <v>100</v>
@@ -7086,7 +7086,7 @@
     </row>
     <row r="36" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="198" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B36" s="199" t="s">
         <v>37</v>
@@ -7095,10 +7095,10 @@
         <v>297</v>
       </c>
       <c r="D36" s="201" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E36" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F36" s="200" t="s">
         <v>77</v>
@@ -7135,11 +7135,11 @@
       <c r="V36" s="61"/>
       <c r="W36" s="150"/>
       <c r="X36" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y36" s="180"/>
       <c r="Z36" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA36" s="211">
         <v>100</v>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="37" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="198" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B37" s="199" t="s">
         <v>37</v>
@@ -7163,10 +7163,10 @@
         <v>297</v>
       </c>
       <c r="D37" s="201" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E37" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F37" s="200" t="s">
         <v>77</v>
@@ -7203,11 +7203,11 @@
       <c r="V37" s="61"/>
       <c r="W37" s="150"/>
       <c r="X37" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y37" s="180"/>
       <c r="Z37" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA37" s="211">
         <v>100</v>
@@ -7222,7 +7222,7 @@
     </row>
     <row r="38" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="198" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B38" s="199" t="s">
         <v>37</v>
@@ -7231,10 +7231,10 @@
         <v>297</v>
       </c>
       <c r="D38" s="201" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E38" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F38" s="200" t="s">
         <v>77</v>
@@ -7271,11 +7271,11 @@
       <c r="V38" s="61"/>
       <c r="W38" s="150"/>
       <c r="X38" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y38" s="180"/>
       <c r="Z38" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA38" s="211">
         <v>100</v>
@@ -7290,7 +7290,7 @@
     </row>
     <row r="39" spans="1:34" ht="25" customHeight="1">
       <c r="A39" s="198" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B39" s="199" t="s">
         <v>37</v>
@@ -7299,10 +7299,10 @@
         <v>297</v>
       </c>
       <c r="D39" s="201" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E39" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F39" s="200" t="s">
         <v>77</v>
@@ -7339,11 +7339,11 @@
       <c r="V39" s="61"/>
       <c r="W39" s="150"/>
       <c r="X39" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y39" s="180"/>
       <c r="Z39" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA39" s="211">
         <v>100</v>
@@ -7358,7 +7358,7 @@
     </row>
     <row r="40" spans="1:34" ht="25" customHeight="1">
       <c r="A40" s="198" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B40" s="199" t="s">
         <v>37</v>
@@ -7367,10 +7367,10 @@
         <v>297</v>
       </c>
       <c r="D40" s="201" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E40" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F40" s="200" t="s">
         <v>77</v>
@@ -7407,11 +7407,11 @@
       <c r="V40" s="61"/>
       <c r="W40" s="150"/>
       <c r="X40" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y40" s="180"/>
       <c r="Z40" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA40" s="211">
         <v>100</v>
@@ -7426,7 +7426,7 @@
     </row>
     <row r="41" spans="1:34" ht="25" customHeight="1">
       <c r="A41" s="198" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B41" s="199" t="s">
         <v>37</v>
@@ -7435,10 +7435,10 @@
         <v>297</v>
       </c>
       <c r="D41" s="201" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E41" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F41" s="200" t="s">
         <v>77</v>
@@ -7475,11 +7475,11 @@
       <c r="V41" s="61"/>
       <c r="W41" s="150"/>
       <c r="X41" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y41" s="180"/>
       <c r="Z41" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA41" s="211">
         <v>100</v>
@@ -7494,7 +7494,7 @@
     </row>
     <row r="42" spans="1:34" ht="25" customHeight="1">
       <c r="A42" s="198" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B42" s="199" t="s">
         <v>37</v>
@@ -7503,10 +7503,10 @@
         <v>297</v>
       </c>
       <c r="D42" s="201" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E42" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F42" s="200" t="s">
         <v>77</v>
@@ -7543,11 +7543,11 @@
       <c r="V42" s="61"/>
       <c r="W42" s="150"/>
       <c r="X42" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y42" s="180"/>
       <c r="Z42" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA42" s="211">
         <v>100</v>
@@ -7562,7 +7562,7 @@
     </row>
     <row r="43" spans="1:34" ht="25" customHeight="1">
       <c r="A43" s="198" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B43" s="199" t="s">
         <v>37</v>
@@ -7571,10 +7571,10 @@
         <v>297</v>
       </c>
       <c r="D43" s="201" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E43" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F43" s="200" t="s">
         <v>77</v>
@@ -7611,11 +7611,11 @@
       <c r="V43" s="61"/>
       <c r="W43" s="150"/>
       <c r="X43" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y43" s="180"/>
       <c r="Z43" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA43" s="211">
         <v>100</v>
@@ -7630,7 +7630,7 @@
     </row>
     <row r="44" spans="1:34" ht="25" customHeight="1">
       <c r="A44" s="198" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B44" s="199" t="s">
         <v>37</v>
@@ -7639,10 +7639,10 @@
         <v>297</v>
       </c>
       <c r="D44" s="201" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E44" s="198" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F44" s="200" t="s">
         <v>77</v>
@@ -7679,11 +7679,11 @@
       <c r="V44" s="61"/>
       <c r="W44" s="150"/>
       <c r="X44" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y44" s="180"/>
       <c r="Z44" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA44" s="211">
         <v>100</v>
@@ -7698,7 +7698,7 @@
     </row>
     <row r="45" spans="1:34" ht="25" customHeight="1">
       <c r="A45" s="198" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B45" s="199" t="s">
         <v>37</v>
@@ -7710,7 +7710,7 @@
         <v>381</v>
       </c>
       <c r="E45" s="198" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F45" s="200" t="s">
         <v>77</v>
@@ -7747,7 +7747,7 @@
       <c r="V45" s="61"/>
       <c r="W45" s="150"/>
       <c r="X45" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y45" s="180"/>
       <c r="Z45" s="212"/>
@@ -7764,7 +7764,7 @@
     </row>
     <row r="46" spans="1:34" ht="25" customHeight="1">
       <c r="A46" s="198" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B46" s="199" t="s">
         <v>37</v>
@@ -7776,7 +7776,7 @@
         <v>382</v>
       </c>
       <c r="E46" s="198" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F46" s="200" t="s">
         <v>77</v>
@@ -7813,7 +7813,7 @@
       <c r="V46" s="61"/>
       <c r="W46" s="150"/>
       <c r="X46" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y46" s="180"/>
       <c r="Z46" s="212"/>
@@ -7830,7 +7830,7 @@
     </row>
     <row r="47" spans="1:34" ht="25" customHeight="1">
       <c r="A47" s="198" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B47" s="199" t="s">
         <v>37</v>
@@ -7842,7 +7842,7 @@
         <v>383</v>
       </c>
       <c r="E47" s="198" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F47" s="200" t="s">
         <v>77</v>
@@ -7879,7 +7879,7 @@
       <c r="V47" s="61"/>
       <c r="W47" s="150"/>
       <c r="X47" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y47" s="180"/>
       <c r="Z47" s="212"/>
@@ -7896,7 +7896,7 @@
     </row>
     <row r="48" spans="1:34" ht="25" customHeight="1">
       <c r="A48" s="198" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B48" s="199" t="s">
         <v>37</v>
@@ -7908,7 +7908,7 @@
         <v>384</v>
       </c>
       <c r="E48" s="198" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F48" s="200" t="s">
         <v>77</v>
@@ -7945,7 +7945,7 @@
       <c r="V48" s="61"/>
       <c r="W48" s="150"/>
       <c r="X48" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y48" s="180"/>
       <c r="Z48" s="212"/>
@@ -7962,7 +7962,7 @@
     </row>
     <row r="49" spans="1:34" ht="25" customHeight="1">
       <c r="A49" s="198" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B49" s="199" t="s">
         <v>37</v>
@@ -7974,7 +7974,7 @@
         <v>385</v>
       </c>
       <c r="E49" s="198" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F49" s="200" t="s">
         <v>77</v>
@@ -8011,7 +8011,7 @@
       <c r="V49" s="61"/>
       <c r="W49" s="150"/>
       <c r="X49" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y49" s="180"/>
       <c r="Z49" s="212"/>
@@ -8028,7 +8028,7 @@
     </row>
     <row r="50" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="205" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B50" s="199" t="s">
         <v>37</v>
@@ -8040,7 +8040,7 @@
         <v>283</v>
       </c>
       <c r="E50" s="198" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F50" s="200" t="s">
         <v>77</v>
@@ -8077,7 +8077,7 @@
       <c r="V50" s="61"/>
       <c r="W50" s="150"/>
       <c r="X50" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y50" s="180"/>
       <c r="Z50" s="212"/>
@@ -8094,7 +8094,7 @@
     </row>
     <row r="51" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="205" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B51" s="199" t="s">
         <v>37</v>
@@ -8106,7 +8106,7 @@
         <v>283</v>
       </c>
       <c r="E51" s="198" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F51" s="200" t="s">
         <v>77</v>
@@ -8143,7 +8143,7 @@
       <c r="V51" s="61"/>
       <c r="W51" s="150"/>
       <c r="X51" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y51" s="180"/>
       <c r="Z51" s="212"/>
@@ -8160,7 +8160,7 @@
     </row>
     <row r="52" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="205" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B52" s="199" t="s">
         <v>37</v>
@@ -8172,7 +8172,7 @@
         <v>283</v>
       </c>
       <c r="E52" s="198" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F52" s="200" t="s">
         <v>77</v>
@@ -8209,7 +8209,7 @@
       <c r="V52" s="61"/>
       <c r="W52" s="150"/>
       <c r="X52" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="Y52" s="180"/>
       <c r="Z52" s="212"/>
@@ -20886,8 +20886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL103"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M40"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20969,7 +20969,7 @@
         <v>352</v>
       </c>
       <c r="P2" s="197" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="Q2" s="42"/>
       <c r="R2" s="6"/>
@@ -21026,7 +21026,7 @@
         <v>298</v>
       </c>
       <c r="K3" s="173" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L3" s="167" t="s">
         <v>27</v>
@@ -21082,7 +21082,7 @@
         <v>299</v>
       </c>
       <c r="K4" s="173" t="s">
-        <v>392</v>
+        <v>513</v>
       </c>
       <c r="L4" s="168" t="s">
         <v>28</v>
@@ -21132,7 +21132,7 @@
         <v>77</v>
       </c>
       <c r="K5" s="196" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L5" s="168" t="s">
         <v>29</v>
@@ -21180,7 +21180,7 @@
         <v>30</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N6" s="175">
         <v>20</v>
@@ -21199,7 +21199,7 @@
     <row r="7" spans="1:38">
       <c r="A7" s="31"/>
       <c r="B7" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>285</v>
@@ -21390,7 +21390,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="20" t="s">
@@ -21428,7 +21428,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="20" t="s">
@@ -21466,7 +21466,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20" t="s">
@@ -21504,7 +21504,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20" t="s">
@@ -21512,7 +21512,7 @@
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="41" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
@@ -21542,7 +21542,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="33"/>
       <c r="C16" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="20" t="s">
@@ -21580,7 +21580,7 @@
       <c r="A17" s="31"/>
       <c r="B17" s="33"/>
       <c r="C17" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20" t="s">
@@ -21616,7 +21616,7 @@
       <c r="A18" s="31"/>
       <c r="B18" s="33"/>
       <c r="C18" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20" t="s">
@@ -21652,7 +21652,7 @@
       <c r="A19" s="31"/>
       <c r="B19" s="33"/>
       <c r="C19" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20" t="s">
@@ -21688,7 +21688,7 @@
       <c r="A20" s="31"/>
       <c r="B20" s="33"/>
       <c r="C20" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20" t="s">
@@ -21724,7 +21724,7 @@
       <c r="A21" s="31"/>
       <c r="B21" s="33"/>
       <c r="C21" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20" t="s">
@@ -21760,7 +21760,7 @@
       <c r="A22" s="31"/>
       <c r="B22" s="33"/>
       <c r="C22" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20" t="s">
@@ -21796,7 +21796,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="33"/>
       <c r="C23" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20" t="s">
@@ -21829,7 +21829,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="33"/>
       <c r="C24" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
@@ -21895,7 +21895,7 @@
       <c r="A26" s="31"/>
       <c r="B26" s="33"/>
       <c r="C26" s="29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="20" t="s">
@@ -21928,7 +21928,7 @@
       <c r="A27" s="31"/>
       <c r="B27" s="33"/>
       <c r="C27" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="20" t="s">
@@ -21961,7 +21961,7 @@
       <c r="A28" s="31"/>
       <c r="B28" s="33"/>
       <c r="C28" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="20" t="s">
@@ -21994,7 +21994,7 @@
       <c r="A29" s="31"/>
       <c r="B29" s="33"/>
       <c r="C29" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="20" t="s">
@@ -22027,7 +22027,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="33"/>
       <c r="C30" s="29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="20" t="s">
@@ -22060,7 +22060,7 @@
       <c r="A31" s="21"/>
       <c r="B31" s="33"/>
       <c r="C31" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="20" t="s">
@@ -22093,7 +22093,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="33"/>
       <c r="C32" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="20" t="s">
@@ -22126,7 +22126,7 @@
       <c r="A33" s="21"/>
       <c r="B33" s="33"/>
       <c r="C33" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="20" t="s">
@@ -22159,7 +22159,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="33"/>
       <c r="C34" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="20" t="s">
@@ -22192,7 +22192,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="33"/>
       <c r="C35" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="20" t="s">

</xml_diff>